<commit_message>
précision définition title bf15cf999fe90ee8dc9b310987b7aeb78d860dd9
</commit_message>
<xml_diff>
--- a/ig/sd-phase-de-lessai-creation-conceptmap/ValueSet-eclaire-study-phase-source-vs.xlsx
+++ b/ig/sd-phase-de-lessai-creation-conceptmap/ValueSet-eclaire-study-phase-source-vs.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Value Set de la phase de l'essai</t>
+    <t>Value Set de la phase de l'essai tel que définie dans la base ECLAIRE</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-31T13:15:07+00:00</t>
+    <t>2023-08-31T14:29:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>